<commit_message>
White and black pipes teleport correctly
</commit_message>
<xml_diff>
--- a/Controle de Horas.xlsx
+++ b/Controle de Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GameMakerStudio2\Stuck in the Sewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEF0291-0E91-4DB1-8768-BA6C5BEE2448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D219227-9600-4928-8887-55CBC27D84C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Início</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Sincronizando Sourcetree</t>
+  </si>
+  <si>
+    <t>Arrumando teleporte dos tubos brancos e pretos</t>
+  </si>
+  <si>
+    <t>Organizando tarefas</t>
   </si>
 </sst>
 </file>
@@ -133,6 +139,9 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <font>
+        <b/>
+      </font>
       <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
@@ -493,11 +502,12 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="43" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="45.7109375" customWidth="1"/>
@@ -587,15 +597,45 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>44902</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>44902</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -800,14 +840,16 @@
   <dimension ref="B1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="64" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="5" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="5"/>
+    <col min="4" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
@@ -840,7 +882,7 @@
       </c>
       <c r="D2" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B2,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>0</v>
+        <v>4.1666666666666685E-2</v>
       </c>
       <c r="E2" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B2,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -850,9 +892,9 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B2,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <f>SUM(C2:F2)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -875,7 +917,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B3,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <f t="shared" ref="G3:G37" si="0">SUM(C3:F3)</f>
         <v>0</v>
       </c>
@@ -900,7 +942,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B4,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -925,7 +967,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B5,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -950,7 +992,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B6,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -975,7 +1017,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B7,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1000,7 +1042,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B8,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1025,7 +1067,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B9,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1050,7 +1092,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B10,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1075,7 +1117,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B11,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1100,7 +1142,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B12,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1125,7 +1167,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B13,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1150,7 +1192,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B14,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1175,7 +1217,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B15,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1200,7 +1242,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B16,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1225,7 +1267,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B17,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1250,7 +1292,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B18,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1275,7 +1317,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B19,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1300,7 +1342,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B20,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1325,7 +1367,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B21,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1350,7 +1392,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B22,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1375,7 +1417,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B23,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1400,7 +1442,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B24,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1425,7 +1467,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B25,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1450,7 +1492,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B26,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1475,7 +1517,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B27,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1500,7 +1542,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B28,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1525,7 +1567,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B29,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1550,7 +1592,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B30,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1575,7 +1617,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B31,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1600,7 +1642,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B32,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1625,7 +1667,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B33,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1650,7 +1692,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B34,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1675,7 +1717,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B35,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1700,7 +1742,7 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B36,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1725,15 +1767,16 @@
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B37,'Folha Ponto'!F:F,Totais!$F$1)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed fade bug; removed "then" keyword
</commit_message>
<xml_diff>
--- a/Controle de Horas.xlsx
+++ b/Controle de Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GameMakerStudio2\Stuck in the Sewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D219227-9600-4928-8887-55CBC27D84C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DACB50A-51A4-4CFF-9D86-5C056D8A6F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Início</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Organizando tarefas</t>
+  </si>
+  <si>
+    <t>Fixed fade bug</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,11 +628,11 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D6" s="3">
-        <v>0.47916666666666669</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>2.083333333333337E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -639,9 +642,24 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>44902</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -882,7 +900,7 @@
       </c>
       <c r="D2" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B2,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>4.1666666666666685E-2</v>
+        <v>7.291666666666663E-2</v>
       </c>
       <c r="E2" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B2,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -894,7 +912,7 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(C2:F2)</f>
-        <v>0.125</v>
+        <v>0.15624999999999994</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented pico font; display coins
</commit_message>
<xml_diff>
--- a/Controle de Horas.xlsx
+++ b/Controle de Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GameMakerStudio2\Stuck in the Sewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DACB50A-51A4-4CFF-9D86-5C056D8A6F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91512FED-8ADF-4502-AB4B-74DA984E212C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Início</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Fixed fade bug</t>
+  </si>
+  <si>
+    <t>Implemented pico font</t>
+  </si>
+  <si>
+    <t>Implemented coin counter display</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,18 +669,45 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>44902</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.5625</v>
+      </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="2">
+        <v>44902</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.57291666666666663</v>
+      </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -900,7 +933,7 @@
       </c>
       <c r="D2" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B2,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>7.291666666666663E-2</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="E2" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B2,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -912,7 +945,7 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(C2:F2)</f>
-        <v>0.15624999999999994</v>
+        <v>0.18749999999999994</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Music, sfx and updated final screen
</commit_message>
<xml_diff>
--- a/Controle de Horas.xlsx
+++ b/Controle de Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GameMakerStudio2\Stuck in the Sewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6306122B-A479-4AF3-8E02-8A03F54BF757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D43A8AD-5AF7-4720-A3BA-0E58FB443E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Início</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Shader aplicado na tela inteira</t>
+  </si>
+  <si>
+    <t>Fazendo descrição do jogo para o Google Play</t>
+  </si>
+  <si>
+    <t>Implementado sons e musica e arrumando tela final</t>
   </si>
 </sst>
 </file>
@@ -153,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -162,6 +168,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,23 +906,66 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="B18" s="2">
+        <v>44904</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.40625</v>
+      </c>
       <c r="E18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.2916666666666685E-2</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>44904</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="E19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>44905</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="E20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -923,6 +973,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
@@ -1099,7 +1150,7 @@
       </c>
       <c r="D4" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B4,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>0</v>
+        <v>0.23958333333333331</v>
       </c>
       <c r="E4" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B4,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -1111,7 +1162,7 @@
       </c>
       <c r="G4" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.23958333333333331</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -1124,7 +1175,7 @@
       </c>
       <c r="D5" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B5,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>0</v>
+        <v>8.3333333333333315E-2</v>
       </c>
       <c r="E5" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B5,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -1136,7 +1187,7 @@
       </c>
       <c r="G5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333315E-2</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ads and icons update
</commit_message>
<xml_diff>
--- a/Controle de Horas.xlsx
+++ b/Controle de Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GameMakerStudio2\Stuck in the Sewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D43A8AD-5AF7-4720-A3BA-0E58FB443E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9666A20B-D0ED-4488-A842-39A59D2762F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>Início</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Implementado sons e musica e arrumando tela final</t>
+  </si>
+  <si>
+    <t>Implementando ads</t>
+  </si>
+  <si>
+    <t>Implementando ads e atualizando loja</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +607,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E22" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E28" si="0">D3-C3</f>
         <v>4.1666666666666685E-2</v>
       </c>
       <c r="F3" t="s">
@@ -969,56 +975,113 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>44905</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="E21" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="6"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="B22" s="2">
+        <v>44905</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.58680555555555558</v>
+      </c>
       <c r="E22" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="B23" s="2">
+        <v>44905</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
@@ -1175,7 +1238,7 @@
       </c>
       <c r="D5" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B5,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="E5" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B5,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -1187,7 +1250,7 @@
       </c>
       <c r="G5" s="4">
         <f t="shared" si="0"/>
-        <v>8.3333333333333315E-2</v>
+        <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New stages with slower progression (green, red and unmixed yellow)
</commit_message>
<xml_diff>
--- a/Controle de Horas.xlsx
+++ b/Controle de Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GameMakerStudio2\Stuck in the Sewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B953EAE-7798-4A1D-A7EF-1869B7728ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DDA82F-A3B4-4C44-97D3-D96F870FEB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
   <si>
     <t>Início</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Arrumando loop da musica</t>
+  </si>
+  <si>
+    <t>Trabalhando em novo level design</t>
   </si>
 </sst>
 </file>
@@ -546,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,23 +1065,46 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="B25" s="2">
+        <v>44906</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.55208333333333337</v>
+      </c>
       <c r="E25" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.11458333333333337</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="B26" s="2">
+        <v>44906</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="E26" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="6"/>
+        <v>0.125</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
@@ -1136,7 +1162,7 @@
   <dimension ref="B1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1304,7 @@
       </c>
       <c r="D6" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B6,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>2.083333333333337E-2</v>
+        <v>0.26041666666666674</v>
       </c>
       <c r="E6" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B6,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -1290,7 +1316,7 @@
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>2.083333333333337E-2</v>
+        <v>0.26041666666666674</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mixed new and old stages in a single run
</commit_message>
<xml_diff>
--- a/Controle de Horas.xlsx
+++ b/Controle de Horas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GameMakerStudio2\Stuck in the Sewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DDA82F-A3B4-4C44-97D3-D96F870FEB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BED64FE-72C0-4B26-B1C1-6C6B4AEBFD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha Ponto" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
   <si>
     <t>Início</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Trabalhando em novo level design</t>
+  </si>
+  <si>
+    <t>Organizando fases e testando</t>
   </si>
 </sst>
 </file>
@@ -549,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,12 +1110,24 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="B27" s="2">
+        <v>44906</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.84375</v>
+      </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -1161,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A44615B-39F7-422F-9D83-BA71A66EE656}">
   <dimension ref="B1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,7 +1319,7 @@
       </c>
       <c r="D6" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B6,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>0.26041666666666674</v>
+        <v>0.31250000000000011</v>
       </c>
       <c r="E6" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B6,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -1316,7 +1331,7 @@
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>0.26041666666666674</v>
+        <v>0.31250000000000011</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented keys, chest, padlocks and new stages
</commit_message>
<xml_diff>
--- a/Controle de Horas.xlsx
+++ b/Controle de Horas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GameMakerStudio2\Stuck in the Sewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BED64FE-72C0-4B26-B1C1-6C6B4AEBFD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A46A1DE-0D80-45CD-8B01-1F17A452EFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha Ponto" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
   <si>
     <t>Início</t>
   </si>
@@ -128,6 +128,24 @@
   </si>
   <si>
     <t>Organizando fases e testando</t>
+  </si>
+  <si>
+    <t>Fazer video tiktok</t>
+  </si>
+  <si>
+    <t>Pesquisar playable ads em HTML5</t>
+  </si>
+  <si>
+    <t>Pesquisando estratégia de marketing</t>
+  </si>
+  <si>
+    <t>Vendo problemas no tiktok e google play</t>
+  </si>
+  <si>
+    <t>Aprendendo a editar videos com programa gratuito</t>
+  </si>
+  <si>
+    <t>Implementando chaves, baús e cadeados</t>
   </si>
 </sst>
 </file>
@@ -192,6 +210,24 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
       </font>
       <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
@@ -226,24 +262,6 @@
       </font>
       <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -258,7 +276,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F23EF26-6211-40DB-A27B-5E91004A4E11}" name="Tabela2" displayName="Tabela2" ref="B1:G1048576" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F23EF26-6211-40DB-A27B-5E91004A4E11}" name="Tabela2" displayName="Tabela2" ref="B1:G1048576" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="B1:G1048576" xr:uid="{3F23EF26-6211-40DB-A27B-5E91004A4E11}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{18BC5966-F532-4B27-8CBD-E1CF183BA466}" name="Data"/>
@@ -273,15 +291,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8AD0E2A5-161A-45D2-B8A8-7FE2E307310A}" name="Tabela3" displayName="Tabela3" ref="B1:G1048576" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8AD0E2A5-161A-45D2-B8A8-7FE2E307310A}" name="Tabela3" displayName="Tabela3" ref="B1:G1048576" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="B1:G1048576" xr:uid="{8AD0E2A5-161A-45D2-B8A8-7FE2E307310A}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BCFA4E1E-0E0E-421A-8B0E-ABF0EFB9E91F}" name="Data"/>
-    <tableColumn id="2" xr3:uid="{E76A3D31-4B88-44BB-B99E-885B305A853C}" name="MMDB" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{967ECFC0-98D8-4902-B332-5DA2E49255E3}" name="SITS" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{B4ABEFEA-D94E-4B59-AE2D-2059C9B4BCEE}" name="Tetris" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{D01DE6DD-BD01-4176-BF6D-3470D6E9390F}" name="Outros" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{AC8C613F-9BE1-4E74-9E6A-1ECD841373B2}" name="Total" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E76A3D31-4B88-44BB-B99E-885B305A853C}" name="MMDB" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{967ECFC0-98D8-4902-B332-5DA2E49255E3}" name="SITS" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{B4ABEFEA-D94E-4B59-AE2D-2059C9B4BCEE}" name="Tetris" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{D01DE6DD-BD01-4176-BF6D-3470D6E9390F}" name="Outros" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{AC8C613F-9BE1-4E74-9E6A-1ECD841373B2}" name="Total" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -550,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G32"/>
+  <dimension ref="B1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +634,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E28" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E43" si="0">D3-C3</f>
         <v>4.1666666666666685E-2</v>
       </c>
       <c r="F3" t="s">
@@ -899,7 +917,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>44903</v>
       </c>
@@ -920,7 +938,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>44904</v>
       </c>
@@ -941,7 +959,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>44904</v>
       </c>
@@ -962,7 +980,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>44905</v>
       </c>
@@ -983,7 +1001,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>44905</v>
       </c>
@@ -1004,7 +1022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>44905</v>
       </c>
@@ -1025,7 +1043,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>44905</v>
       </c>
@@ -1046,7 +1064,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>44906</v>
       </c>
@@ -1067,7 +1085,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>44906</v>
       </c>
@@ -1088,7 +1106,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>44906</v>
       </c>
@@ -1109,7 +1127,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>44906</v>
       </c>
@@ -1130,38 +1148,227 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>44907</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="E28" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>44907</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>44908</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>44908</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>44908</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>44909</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>44909</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="0"/>
+        <v>9.027777777777779E-2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>44909</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="0"/>
+        <v>0.21527777777777779</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E36" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E38" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E39" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1176,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A44615B-39F7-422F-9D83-BA71A66EE656}">
   <dimension ref="B1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,11 +1559,11 @@
       </c>
       <c r="F7" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B7,'Folha Ponto'!F:F,Totais!$F$1)</f>
-        <v>0</v>
+        <v>0.12500000000000006</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.12500000000000006</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -1369,7 +1576,7 @@
       </c>
       <c r="D8" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B8,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>0</v>
+        <v>0.20833333333333326</v>
       </c>
       <c r="E8" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B8,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -1377,11 +1584,11 @@
       </c>
       <c r="F8" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B8,'Folha Ponto'!F:F,Totais!$F$1)</f>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.29166666666666663</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1394,7 +1601,7 @@
       </c>
       <c r="D9" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B9,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>0</v>
+        <v>0.38888888888888895</v>
       </c>
       <c r="E9" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B9,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -1406,7 +1613,7 @@
       </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.38888888888888895</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More stages (all old ones are included now)
</commit_message>
<xml_diff>
--- a/Controle de Horas.xlsx
+++ b/Controle de Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GameMakerStudio2\Stuck in the Sewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A46A1DE-0D80-45CD-8B01-1F17A452EFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DE955D-5958-4346-AF62-A40529D5CA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
   <si>
     <t>Início</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Implementando chaves, baús e cadeados</t>
+  </si>
+  <si>
+    <t>Implementando fases novas</t>
+  </si>
+  <si>
+    <t>Brainstorm de nomes pra empresa e jogos</t>
   </si>
 </sst>
 </file>
@@ -210,24 +216,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
       </font>
       <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
@@ -262,6 +250,24 @@
       </font>
       <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -276,7 +282,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F23EF26-6211-40DB-A27B-5E91004A4E11}" name="Tabela2" displayName="Tabela2" ref="B1:G1048576" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F23EF26-6211-40DB-A27B-5E91004A4E11}" name="Tabela2" displayName="Tabela2" ref="B1:G1048576" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="B1:G1048576" xr:uid="{3F23EF26-6211-40DB-A27B-5E91004A4E11}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{18BC5966-F532-4B27-8CBD-E1CF183BA466}" name="Data"/>
@@ -291,15 +297,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8AD0E2A5-161A-45D2-B8A8-7FE2E307310A}" name="Tabela3" displayName="Tabela3" ref="B1:G1048576" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8AD0E2A5-161A-45D2-B8A8-7FE2E307310A}" name="Tabela3" displayName="Tabela3" ref="B1:G1048576" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="B1:G1048576" xr:uid="{8AD0E2A5-161A-45D2-B8A8-7FE2E307310A}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BCFA4E1E-0E0E-421A-8B0E-ABF0EFB9E91F}" name="Data"/>
-    <tableColumn id="2" xr3:uid="{E76A3D31-4B88-44BB-B99E-885B305A853C}" name="MMDB" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{967ECFC0-98D8-4902-B332-5DA2E49255E3}" name="SITS" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{B4ABEFEA-D94E-4B59-AE2D-2059C9B4BCEE}" name="Tetris" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{D01DE6DD-BD01-4176-BF6D-3470D6E9390F}" name="Outros" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{AC8C613F-9BE1-4E74-9E6A-1ECD841373B2}" name="Total" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E76A3D31-4B88-44BB-B99E-885B305A853C}" name="MMDB" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{967ECFC0-98D8-4902-B332-5DA2E49255E3}" name="SITS" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{B4ABEFEA-D94E-4B59-AE2D-2059C9B4BCEE}" name="Tetris" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D01DE6DD-BD01-4176-BF6D-3470D6E9390F}" name="Outros" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{AC8C613F-9BE1-4E74-9E6A-1ECD841373B2}" name="Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -571,7 +577,7 @@
   <dimension ref="B1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,33 +1329,108 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>44909</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.375</v>
+      </c>
       <c r="E36" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>44909</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.5</v>
+      </c>
       <c r="E37" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <v>44909</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.53125</v>
+      </c>
       <c r="E38" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <v>44909</v>
+      </c>
+      <c r="C39" s="8">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E39" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.11458333333333326</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <v>44909</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.71875</v>
+      </c>
       <c r="E40" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
@@ -1601,7 +1682,7 @@
       </c>
       <c r="D9" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B9,'Folha Ponto'!F:F,Totais!$D$1)</f>
-        <v>0.38888888888888895</v>
+        <v>0.62847222222222221</v>
       </c>
       <c r="E9" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B9,'Folha Ponto'!F:F,Totais!$E$1)</f>
@@ -1609,11 +1690,11 @@
       </c>
       <c r="F9" s="5">
         <f>SUMIFS('Folha Ponto'!E:E,'Folha Ponto'!B:B,Totais!B9,'Folha Ponto'!F:F,Totais!$F$1)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>0.38888888888888895</v>
+        <v>0.75347222222222221</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>